<commit_message>
Modificaciones pedididas por los profesores el viernes pasado
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/Matriz de Costos/Plantilla Estimación de Costos v1.0.xlsx
+++ b/trunk/docs/Entregables/Matriz de Costos/Plantilla Estimación de Costos v1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimación de Costos" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
   <si>
     <t>Estimación de Costos</t>
   </si>
@@ -372,6 +372,9 @@
   <si>
     <t>Expensas</t>
   </si>
+  <si>
+    <t>TOTAL Mensual</t>
+  </si>
 </sst>
 </file>
 
@@ -492,7 +495,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,8 +544,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -988,6 +997,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -995,7 +1028,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1193,6 +1226,8 @@
     <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="28" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1231,8 +1266,18 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="28" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moneda" xfId="3" builtinId="4"/>
@@ -1265,7 +1310,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1308,7 +1353,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1612,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1001"/>
+  <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1630,22 +1675,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="85"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="87"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1657,11 +1702,11 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
       <c r="D2" s="78"/>
       <c r="E2" s="75" t="s">
         <v>69</v>
@@ -1704,10 +1749,10 @@
       <c r="W2" s="4"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="83" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1715,40 +1760,40 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="80">
-        <f>RRHH!C34</f>
-        <v>274952.32800000004</v>
+        <f>RRHH!C35</f>
+        <v>193628.4</v>
       </c>
       <c r="F3" s="80">
-        <f>RRHH!D34</f>
-        <v>274952.32800000004</v>
+        <f>RRHH!D35</f>
+        <v>193628.4</v>
       </c>
       <c r="G3" s="80">
-        <f>RRHH!E34</f>
-        <v>274952.32800000004</v>
+        <f>RRHH!E35</f>
+        <v>242035.5</v>
       </c>
       <c r="H3" s="80">
-        <f>RRHH!F34</f>
-        <v>305932.87199999997</v>
+        <f>RRHH!F35</f>
+        <v>360148.82399999996</v>
       </c>
       <c r="I3" s="80">
-        <f>RRHH!G34</f>
-        <v>249780.636</v>
+        <f>RRHH!G35</f>
+        <v>303996.58799999999</v>
       </c>
       <c r="J3" s="80">
-        <f>RRHH!H34</f>
-        <v>249780.636</v>
+        <f>RRHH!H35</f>
+        <v>303996.58799999999</v>
       </c>
       <c r="K3" s="80">
-        <f>RRHH!I34</f>
-        <v>249780.636</v>
+        <f>RRHH!I35</f>
+        <v>303996.58799999999</v>
       </c>
       <c r="L3" s="80">
-        <f>RRHH!J34</f>
-        <v>249780.636</v>
+        <f>RRHH!J35</f>
+        <v>303996.58799999999</v>
       </c>
       <c r="M3" s="80">
-        <f>RRHH!K34</f>
-        <v>218800.092</v>
+        <f>RRHH!K35</f>
+        <v>273016.04399999999</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="8"/>
@@ -1761,46 +1806,46 @@
       <c r="V3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="90"/>
-      <c r="B4" s="88"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="90"/>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="80">
-        <f>RRHH!B35</f>
+        <f>RRHH!B36</f>
         <v>0</v>
       </c>
       <c r="F4" s="80">
-        <f>RRHH!C35</f>
+        <f>RRHH!C36</f>
         <v>0</v>
       </c>
       <c r="G4" s="80">
-        <f>RRHH!D35</f>
+        <f>RRHH!D36</f>
         <v>0</v>
       </c>
       <c r="H4" s="80">
-        <f>RRHH!E35</f>
-        <v>48407.1</v>
+        <f>RRHH!E36</f>
+        <v>40000</v>
       </c>
       <c r="I4" s="80">
-        <f>RRHH!F35</f>
-        <v>48407.1</v>
+        <f>RRHH!F36</f>
+        <v>40000</v>
       </c>
       <c r="J4" s="80">
-        <f>RRHH!G35</f>
-        <v>48407.1</v>
+        <f>RRHH!G36</f>
+        <v>40000</v>
       </c>
       <c r="K4" s="80">
-        <f>RRHH!H35</f>
-        <v>48407.1</v>
+        <f>RRHH!H36</f>
+        <v>40000</v>
       </c>
       <c r="L4" s="80">
-        <f>RRHH!I35</f>
+        <f>RRHH!I36</f>
         <v>0</v>
       </c>
       <c r="M4" s="80">
-        <f>RRHH!J35</f>
+        <f>RRHH!J36</f>
         <v>0</v>
       </c>
       <c r="N4" s="6"/>
@@ -1814,8 +1859,8 @@
       <c r="V4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="90"/>
-      <c r="B5" s="81" t="s">
+      <c r="A5" s="92"/>
+      <c r="B5" s="83" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1842,8 +1887,8 @@
       <c r="V5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="90"/>
-      <c r="B6" s="88"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1868,8 +1913,8 @@
       <c r="V6" s="9"/>
     </row>
     <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="90"/>
-      <c r="B7" s="81" t="s">
+      <c r="A7" s="92"/>
+      <c r="B7" s="83" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1896,8 +1941,8 @@
       <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
-      <c r="B8" s="88"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1922,8 +1967,8 @@
       <c r="V8" s="9"/>
     </row>
     <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
-      <c r="B9" s="81" t="s">
+      <c r="A9" s="92"/>
+      <c r="B9" s="83" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1950,8 +1995,8 @@
       <c r="V9" s="9"/>
     </row>
     <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1994,7 +2039,7 @@
       <c r="V10" s="9"/>
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="90"/>
+      <c r="A11" s="92"/>
       <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
@@ -2042,8 +2087,8 @@
       <c r="V11" s="9"/>
     </row>
     <row r="12" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
-      <c r="B12" s="81" t="s">
+      <c r="A12" s="92"/>
+      <c r="B12" s="83" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -2088,8 +2133,8 @@
       <c r="V12" s="12"/>
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="90"/>
-      <c r="B13" s="82"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="5" t="s">
         <v>110</v>
       </c>
@@ -2141,10 +2186,10 @@
       <c r="V13" s="12"/>
     </row>
     <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="83" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -2171,8 +2216,8 @@
       <c r="V14" s="9"/>
     </row>
     <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="90"/>
-      <c r="B15" s="88"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
@@ -2197,8 +2242,8 @@
       <c r="V15" s="9"/>
     </row>
     <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
-      <c r="B16" s="81" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="83" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -2225,8 +2270,8 @@
       <c r="V16" s="9"/>
     </row>
     <row r="17" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="90"/>
-      <c r="B17" s="88"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="5" t="s">
         <v>27</v>
       </c>
@@ -2251,8 +2296,8 @@
       <c r="V17" s="9"/>
     </row>
     <row r="18" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="81" t="s">
+      <c r="A18" s="92"/>
+      <c r="B18" s="83" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -2279,8 +2324,8 @@
       <c r="V18" s="9"/>
     </row>
     <row r="19" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="90"/>
-      <c r="B19" s="88"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="5" t="s">
         <v>31</v>
       </c>
@@ -2305,8 +2350,8 @@
       <c r="V19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="90"/>
-      <c r="B20" s="81" t="s">
+      <c r="A20" s="92"/>
+      <c r="B20" s="83" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -2333,8 +2378,8 @@
       <c r="V20" s="9"/>
     </row>
     <row r="21" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="90"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="5" t="s">
         <v>27</v>
       </c>
@@ -2359,8 +2404,8 @@
       <c r="V21" s="9"/>
     </row>
     <row r="22" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="90"/>
-      <c r="B22" s="81" t="s">
+      <c r="A22" s="92"/>
+      <c r="B22" s="83" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -2387,8 +2432,8 @@
       <c r="V22" s="9"/>
     </row>
     <row r="23" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="90"/>
-      <c r="B23" s="88"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="5" t="s">
         <v>27</v>
       </c>
@@ -2413,8 +2458,8 @@
       <c r="V23" s="9"/>
     </row>
     <row r="24" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="90"/>
-      <c r="B24" s="81" t="s">
+      <c r="A24" s="92"/>
+      <c r="B24" s="83" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -2441,8 +2486,8 @@
       <c r="V24" s="9"/>
     </row>
     <row r="25" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="90"/>
       <c r="C25" s="5" t="s">
         <v>31</v>
       </c>
@@ -2504,18 +2549,45 @@
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="57" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
+      <c r="E28" s="57">
+        <f>SUM(E3:E26)</f>
+        <v>301628.40000000002</v>
+      </c>
+      <c r="F28" s="57">
+        <f t="shared" ref="F28:L28" si="0">SUM(F3:F26)</f>
+        <v>301628.40000000002</v>
+      </c>
+      <c r="G28" s="57">
+        <f t="shared" si="0"/>
+        <v>350035.5</v>
+      </c>
+      <c r="H28" s="57">
+        <f t="shared" si="0"/>
+        <v>508148.82399999996</v>
+      </c>
+      <c r="I28" s="57">
+        <f t="shared" si="0"/>
+        <v>451996.58799999999</v>
+      </c>
+      <c r="J28" s="57">
+        <f t="shared" si="0"/>
+        <v>451996.58799999999</v>
+      </c>
+      <c r="K28" s="57">
+        <f t="shared" si="0"/>
+        <v>451996.58799999999</v>
+      </c>
+      <c r="L28" s="57">
+        <f t="shared" si="0"/>
+        <v>411996.58799999999</v>
+      </c>
+      <c r="M28" s="57">
+        <f>SUM(M3:M26)</f>
+        <v>381016.04399999999</v>
+      </c>
       <c r="N28" s="9"/>
     </row>
     <row r="29" spans="1:22" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2525,15 +2597,42 @@
         <v>36</v>
       </c>
       <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="57"/>
+      <c r="E29" s="57">
+        <f>E28</f>
+        <v>301628.40000000002</v>
+      </c>
+      <c r="F29" s="57">
+        <f>E29+F28</f>
+        <v>603256.80000000005</v>
+      </c>
+      <c r="G29" s="57">
+        <f>F29+G28</f>
+        <v>953292.3</v>
+      </c>
+      <c r="H29" s="57">
+        <f t="shared" ref="H29:M29" si="1">G29+H28</f>
+        <v>1461441.1240000001</v>
+      </c>
+      <c r="I29" s="57">
+        <f t="shared" si="1"/>
+        <v>1913437.7120000001</v>
+      </c>
+      <c r="J29" s="57">
+        <f t="shared" si="1"/>
+        <v>2365434.2999999998</v>
+      </c>
+      <c r="K29" s="57">
+        <f t="shared" si="1"/>
+        <v>2817430.8879999998</v>
+      </c>
+      <c r="L29" s="57">
+        <f t="shared" si="1"/>
+        <v>3229427.4759999998</v>
+      </c>
+      <c r="M29" s="100">
+        <f t="shared" si="1"/>
+        <v>3610443.5199999996</v>
+      </c>
       <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2553,9 +2652,9 @@
       <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -2566,7 +2665,7 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
-      <c r="N31" s="9"/>
+      <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
@@ -18071,22 +18170,6 @@
       <c r="L1000" s="11"/>
       <c r="M1000" s="11"/>
       <c r="N1000" s="12"/>
-    </row>
-    <row r="1001" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1001" s="12"/>
-      <c r="B1001" s="12"/>
-      <c r="C1001" s="12"/>
-      <c r="D1001" s="12"/>
-      <c r="E1001" s="11"/>
-      <c r="F1001" s="11"/>
-      <c r="G1001" s="11"/>
-      <c r="H1001" s="11"/>
-      <c r="I1001" s="11"/>
-      <c r="J1001" s="11"/>
-      <c r="K1001" s="11"/>
-      <c r="L1001" s="11"/>
-      <c r="M1001" s="11"/>
-      <c r="N1001" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -18113,10 +18196,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K38"/>
+  <dimension ref="A2:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18368,36 +18451,15 @@
       <c r="A10" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="17">
-        <v>25000</v>
-      </c>
-      <c r="C10" s="18">
-        <f t="shared" si="0"/>
-        <v>12000</v>
-      </c>
-      <c r="D10" s="20">
-        <f t="shared" si="1"/>
-        <v>37000</v>
-      </c>
-      <c r="E10" s="19">
-        <f t="shared" si="2"/>
-        <v>3082.1</v>
-      </c>
-      <c r="F10" s="19">
-        <f t="shared" si="3"/>
-        <v>3082.1</v>
-      </c>
-      <c r="G10" s="19">
-        <f t="shared" si="4"/>
-        <v>3700</v>
-      </c>
-      <c r="H10" s="19">
-        <f t="shared" si="5"/>
-        <v>1542.9</v>
-      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
       <c r="I10" s="53">
-        <f t="shared" si="6"/>
-        <v>48407.1</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -18514,35 +18576,35 @@
       </c>
       <c r="B14" s="56">
         <f>SUM(B5:B13)</f>
-        <v>211000</v>
+        <v>186000</v>
       </c>
       <c r="C14" s="57">
         <f t="shared" ref="C14:I14" si="8">SUM(C5:C13)</f>
-        <v>101280</v>
+        <v>89280</v>
       </c>
       <c r="D14" s="56">
         <f t="shared" si="8"/>
-        <v>312280</v>
+        <v>275280</v>
       </c>
       <c r="E14" s="56">
         <f t="shared" si="8"/>
-        <v>26012.923999999999</v>
+        <v>22930.824000000001</v>
       </c>
       <c r="F14" s="56">
         <f t="shared" si="8"/>
-        <v>26012.923999999999</v>
+        <v>22930.824000000001</v>
       </c>
       <c r="G14" s="56">
         <f t="shared" si="8"/>
-        <v>31228</v>
+        <v>27528</v>
       </c>
       <c r="H14" s="56">
         <f t="shared" si="8"/>
-        <v>13022.075999999997</v>
+        <v>11479.175999999999</v>
       </c>
       <c r="I14" s="58">
         <f t="shared" si="8"/>
-        <v>408555.92399999994</v>
+        <v>400148.82399999996</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -18671,17 +18733,17 @@
       <c r="B26" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="98"/>
+      <c r="K26" s="99"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
@@ -18764,95 +18826,89 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="33">
         <v>0</v>
       </c>
       <c r="C29" s="36">
-        <f>$I$7</f>
-        <v>48407.1</v>
+        <f>$I$6</f>
+        <v>54215.951999999997</v>
       </c>
       <c r="D29" s="36">
-        <f t="shared" ref="D29:K29" si="10">$I$7</f>
-        <v>48407.1</v>
+        <f t="shared" ref="D29:K29" si="10">$I$6</f>
+        <v>54215.951999999997</v>
       </c>
       <c r="E29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
       <c r="F29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
       <c r="G29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
       <c r="H29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
       <c r="I29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
       <c r="J29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
       <c r="K29" s="36">
         <f t="shared" si="10"/>
-        <v>48407.1</v>
+        <v>54215.951999999997</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B30" s="33">
         <v>0</v>
       </c>
-      <c r="C30" s="36">
-        <f>$I$8+$I$9</f>
-        <v>87132.78</v>
-      </c>
-      <c r="D30" s="36">
-        <f t="shared" ref="D30:K30" si="11">$I$8+$I$9</f>
-        <v>87132.78</v>
-      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
       <c r="E30" s="36">
-        <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <f t="shared" ref="D30:K30" si="11">$I$7</f>
+        <v>48407.1</v>
       </c>
       <c r="F30" s="36">
         <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <v>48407.1</v>
       </c>
       <c r="G30" s="36">
         <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <v>48407.1</v>
       </c>
       <c r="H30" s="36">
         <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <v>48407.1</v>
       </c>
       <c r="I30" s="36">
         <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <v>48407.1</v>
       </c>
       <c r="J30" s="36">
         <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <v>48407.1</v>
       </c>
       <c r="K30" s="36">
         <f t="shared" si="11"/>
-        <v>87132.78</v>
+        <v>48407.1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B31" s="33">
         <v>0</v>
@@ -18861,282 +18917,318 @@
       <c r="D31" s="36"/>
       <c r="E31" s="36"/>
       <c r="F31" s="36">
+        <f t="shared" ref="D31:K31" si="12">$I$8+$I$9</f>
+        <v>87132.78</v>
+      </c>
+      <c r="G31" s="36">
+        <f t="shared" si="12"/>
+        <v>87132.78</v>
+      </c>
+      <c r="H31" s="36">
+        <f t="shared" si="12"/>
+        <v>87132.78</v>
+      </c>
+      <c r="I31" s="36">
+        <f t="shared" si="12"/>
+        <v>87132.78</v>
+      </c>
+      <c r="J31" s="36">
+        <f t="shared" si="12"/>
+        <v>87132.78</v>
+      </c>
+      <c r="K31" s="36">
+        <f t="shared" si="12"/>
+        <v>87132.78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="33">
+        <v>0</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36">
         <f>$I$11</f>
         <v>30980.544000000002</v>
       </c>
-      <c r="G31" s="36">
-        <f t="shared" ref="G31:J31" si="12">$I$11</f>
+      <c r="G32" s="36">
+        <f t="shared" ref="G32:J32" si="13">$I$11</f>
         <v>30980.544000000002</v>
       </c>
-      <c r="H31" s="36">
-        <f t="shared" si="12"/>
+      <c r="H32" s="36">
+        <f t="shared" si="13"/>
         <v>30980.544000000002</v>
       </c>
-      <c r="I31" s="36">
-        <f t="shared" si="12"/>
+      <c r="I32" s="36">
+        <f t="shared" si="13"/>
         <v>30980.544000000002</v>
       </c>
-      <c r="J31" s="36">
-        <f t="shared" si="12"/>
+      <c r="J32" s="36">
+        <f t="shared" si="13"/>
         <v>30980.544000000002</v>
       </c>
-      <c r="K31" s="36"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="30" t="s">
+      <c r="K32" s="36"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="33">
+      <c r="B33" s="33">
         <v>0</v>
       </c>
-      <c r="C32" s="36">
+      <c r="C33" s="36">
         <f>$I$12</f>
         <v>56152.235999999997</v>
       </c>
-      <c r="D32" s="36">
-        <f t="shared" ref="D32:F32" si="13">$I$12</f>
+      <c r="D33" s="36">
+        <f t="shared" ref="D33:F33" si="14">$I$12</f>
         <v>56152.235999999997</v>
       </c>
-      <c r="E32" s="36">
-        <f t="shared" si="13"/>
+      <c r="E33" s="36">
+        <f t="shared" si="14"/>
         <v>56152.235999999997</v>
       </c>
-      <c r="F32" s="36">
-        <f t="shared" si="13"/>
+      <c r="F33" s="36">
+        <f t="shared" si="14"/>
         <v>56152.235999999997</v>
       </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="30" t="s">
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="33">
+      <c r="B34" s="33">
         <v>0</v>
       </c>
-      <c r="C33" s="36">
+      <c r="C34" s="36">
         <f>$I$13</f>
         <v>15490.272000000001</v>
       </c>
-      <c r="D33" s="36">
-        <f t="shared" ref="D33:K33" si="14">$I$13</f>
+      <c r="D34" s="36">
+        <f t="shared" ref="D34:K34" si="15">$I$13</f>
         <v>15490.272000000001</v>
       </c>
-      <c r="E33" s="36">
-        <f t="shared" si="14"/>
+      <c r="E34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
-      <c r="F33" s="36">
-        <f t="shared" si="14"/>
+      <c r="F34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
-      <c r="G33" s="36">
-        <f t="shared" si="14"/>
+      <c r="G34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
-      <c r="H33" s="36">
-        <f t="shared" si="14"/>
+      <c r="H34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
-      <c r="I33" s="36">
-        <f t="shared" si="14"/>
+      <c r="I34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
-      <c r="J33" s="36">
-        <f t="shared" si="14"/>
+      <c r="J34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
-      <c r="K33" s="36">
-        <f t="shared" si="14"/>
+      <c r="K34" s="36">
+        <f t="shared" si="15"/>
         <v>15490.272000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="34" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="35">
+      <c r="B35" s="35">
         <v>0</v>
       </c>
-      <c r="C34" s="37">
-        <f t="shared" ref="C34:K34" si="15">SUM(C28:C33)</f>
-        <v>274952.32800000004</v>
-      </c>
-      <c r="D34" s="37">
-        <f t="shared" si="15"/>
-        <v>274952.32800000004</v>
-      </c>
-      <c r="E34" s="37">
-        <f t="shared" si="15"/>
-        <v>274952.32800000004</v>
-      </c>
-      <c r="F34" s="37">
-        <f t="shared" si="15"/>
-        <v>305932.87199999997</v>
-      </c>
-      <c r="G34" s="37">
-        <f t="shared" si="15"/>
-        <v>249780.636</v>
-      </c>
-      <c r="H34" s="37">
-        <f t="shared" si="15"/>
-        <v>249780.636</v>
-      </c>
-      <c r="I34" s="37">
-        <f t="shared" si="15"/>
-        <v>249780.636</v>
-      </c>
-      <c r="J34" s="37">
-        <f t="shared" si="15"/>
-        <v>249780.636</v>
-      </c>
-      <c r="K34" s="38">
-        <f t="shared" si="15"/>
-        <v>218800.092</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+      <c r="C35" s="37">
+        <f t="shared" ref="C35:K35" si="16">SUM(C28:C34)</f>
+        <v>193628.4</v>
+      </c>
+      <c r="D35" s="37">
+        <f t="shared" si="16"/>
+        <v>193628.4</v>
+      </c>
+      <c r="E35" s="37">
+        <f t="shared" si="16"/>
+        <v>242035.5</v>
+      </c>
+      <c r="F35" s="37">
+        <f t="shared" si="16"/>
+        <v>360148.82399999996</v>
+      </c>
+      <c r="G35" s="37">
+        <f t="shared" si="16"/>
+        <v>303996.58799999999</v>
+      </c>
+      <c r="H35" s="37">
+        <f t="shared" si="16"/>
+        <v>303996.58799999999</v>
+      </c>
+      <c r="I35" s="37">
+        <f t="shared" si="16"/>
+        <v>303996.58799999999</v>
+      </c>
+      <c r="J35" s="37">
+        <f t="shared" si="16"/>
+        <v>303996.58799999999</v>
+      </c>
+      <c r="K35" s="38">
+        <f t="shared" si="16"/>
+        <v>273016.04399999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36">
+      <c r="B36" s="33"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36">
         <f>$I$10</f>
-        <v>48407.1</v>
-      </c>
-      <c r="F35" s="36">
-        <f t="shared" ref="F35:H35" si="16">$I$10</f>
-        <v>48407.1</v>
-      </c>
-      <c r="G35" s="36">
-        <f t="shared" si="16"/>
-        <v>48407.1</v>
-      </c>
-      <c r="H35" s="36">
-        <f t="shared" si="16"/>
-        <v>48407.1</v>
-      </c>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="34" t="s">
+        <v>40000</v>
+      </c>
+      <c r="F36" s="36">
+        <f t="shared" ref="F36:H36" si="17">$I$10</f>
+        <v>40000</v>
+      </c>
+      <c r="G36" s="36">
+        <f t="shared" si="17"/>
+        <v>40000</v>
+      </c>
+      <c r="H36" s="36">
+        <f t="shared" si="17"/>
+        <v>40000</v>
+      </c>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="40">
-        <f>SUM(B35)</f>
+      <c r="B37" s="40">
+        <f>SUM(B36)</f>
         <v>0</v>
       </c>
-      <c r="C36" s="40">
-        <f t="shared" ref="C36:K36" si="17">SUM(C35)</f>
+      <c r="C37" s="40">
+        <f t="shared" ref="C37:K37" si="18">SUM(C36)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="40">
-        <f t="shared" si="17"/>
+      <c r="D37" s="40">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="E36" s="40">
-        <f t="shared" si="17"/>
-        <v>48407.1</v>
-      </c>
-      <c r="F36" s="40">
-        <f t="shared" si="17"/>
-        <v>48407.1</v>
-      </c>
-      <c r="G36" s="40">
-        <f t="shared" si="17"/>
-        <v>48407.1</v>
-      </c>
-      <c r="H36" s="40">
-        <f t="shared" si="17"/>
-        <v>48407.1</v>
-      </c>
-      <c r="I36" s="40">
-        <f t="shared" si="17"/>
+      <c r="E37" s="40">
+        <f t="shared" si="18"/>
+        <v>40000</v>
+      </c>
+      <c r="F37" s="40">
+        <f t="shared" si="18"/>
+        <v>40000</v>
+      </c>
+      <c r="G37" s="40">
+        <f t="shared" si="18"/>
+        <v>40000</v>
+      </c>
+      <c r="H37" s="40">
+        <f t="shared" si="18"/>
+        <v>40000</v>
+      </c>
+      <c r="I37" s="40">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="J36" s="40">
-        <f t="shared" si="17"/>
+      <c r="J37" s="40">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="K36" s="40">
-        <f t="shared" si="17"/>
+      <c r="K37" s="40">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+    <row r="38" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="41">
-        <f>B34+B36</f>
+      <c r="B38" s="41">
+        <f>B35+B37</f>
         <v>0</v>
       </c>
-      <c r="C37" s="41">
-        <f t="shared" ref="C37:K37" si="18">C34+C36</f>
-        <v>274952.32800000004</v>
-      </c>
-      <c r="D37" s="41">
-        <f t="shared" si="18"/>
-        <v>274952.32800000004</v>
-      </c>
-      <c r="E37" s="41">
-        <f t="shared" si="18"/>
-        <v>323359.42800000001</v>
-      </c>
-      <c r="F37" s="41">
-        <f t="shared" si="18"/>
-        <v>354339.97199999995</v>
-      </c>
-      <c r="G37" s="41">
-        <f t="shared" si="18"/>
-        <v>298187.73599999998</v>
-      </c>
-      <c r="H37" s="41">
-        <f t="shared" si="18"/>
-        <v>298187.73599999998</v>
-      </c>
-      <c r="I37" s="41">
-        <f t="shared" si="18"/>
-        <v>249780.636</v>
-      </c>
-      <c r="J37" s="41">
-        <f t="shared" si="18"/>
-        <v>249780.636</v>
-      </c>
-      <c r="K37" s="41">
-        <f t="shared" si="18"/>
-        <v>218800.092</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="91" t="s">
+      <c r="C38" s="41">
+        <f t="shared" ref="C38:K38" si="19">C35+C37</f>
+        <v>193628.4</v>
+      </c>
+      <c r="D38" s="41">
+        <f t="shared" si="19"/>
+        <v>193628.4</v>
+      </c>
+      <c r="E38" s="41">
+        <f t="shared" si="19"/>
+        <v>282035.5</v>
+      </c>
+      <c r="F38" s="41">
+        <f t="shared" si="19"/>
+        <v>400148.82399999996</v>
+      </c>
+      <c r="G38" s="41">
+        <f t="shared" si="19"/>
+        <v>343996.58799999999</v>
+      </c>
+      <c r="H38" s="41">
+        <f t="shared" si="19"/>
+        <v>343996.58799999999</v>
+      </c>
+      <c r="I38" s="41">
+        <f t="shared" si="19"/>
+        <v>303996.58799999999</v>
+      </c>
+      <c r="J38" s="41">
+        <f t="shared" si="19"/>
+        <v>303996.58799999999</v>
+      </c>
+      <c r="K38" s="41">
+        <f t="shared" si="19"/>
+        <v>273016.04399999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="91"/>
-      <c r="H38" s="91"/>
-      <c r="I38" s="91"/>
-      <c r="J38" s="92"/>
-      <c r="K38" s="42">
-        <f>SUM(C34:K34)</f>
-        <v>2348712.4920000001</v>
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="42">
+        <f>SUM(C35:K35)</f>
+        <v>2478443.5199999996</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A38:J38"/>
+  <mergeCells count="2">
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="C26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -19223,10 +19315,10 @@
       <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="93"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="48">
         <f>SUM(C3:C8)</f>
         <v>210000</v>
@@ -19244,7 +19336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -19293,7 +19385,7 @@
       <c r="C4" s="61">
         <v>5</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="81">
         <f t="shared" ref="D4:D17" si="0">B4*C4</f>
         <v>7500</v>
       </c>
@@ -19308,7 +19400,7 @@
       <c r="C5" s="61">
         <v>1</v>
       </c>
-      <c r="D5" s="96">
+      <c r="D5" s="82">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
@@ -19323,7 +19415,7 @@
       <c r="C6" s="61">
         <v>1</v>
       </c>
-      <c r="D6" s="96">
+      <c r="D6" s="82">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
@@ -19338,7 +19430,7 @@
       <c r="C7" s="61">
         <v>1</v>
       </c>
-      <c r="D7" s="96">
+      <c r="D7" s="82">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
@@ -19353,7 +19445,7 @@
       <c r="C8" s="61">
         <v>1</v>
       </c>
-      <c r="D8" s="96">
+      <c r="D8" s="82">
         <f t="shared" si="0"/>
         <v>4200</v>
       </c>
@@ -19368,7 +19460,7 @@
       <c r="C9" s="61">
         <v>1</v>
       </c>
-      <c r="D9" s="96">
+      <c r="D9" s="82">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
@@ -19383,7 +19475,7 @@
       <c r="C10" s="61">
         <v>5</v>
       </c>
-      <c r="D10" s="96">
+      <c r="D10" s="82">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
@@ -19398,7 +19490,7 @@
       <c r="C11" s="61">
         <v>1</v>
       </c>
-      <c r="D11" s="96">
+      <c r="D11" s="82">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
@@ -19413,7 +19505,7 @@
       <c r="C12" s="61">
         <v>1</v>
       </c>
-      <c r="D12" s="96">
+      <c r="D12" s="82">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
@@ -19428,7 +19520,7 @@
       <c r="C13" s="61">
         <v>5</v>
       </c>
-      <c r="D13" s="96">
+      <c r="D13" s="82">
         <f t="shared" si="0"/>
         <v>3500</v>
       </c>
@@ -19443,7 +19535,7 @@
       <c r="C14" s="61">
         <v>1</v>
       </c>
-      <c r="D14" s="96">
+      <c r="D14" s="82">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
@@ -19458,7 +19550,7 @@
       <c r="C15" s="61">
         <v>5</v>
       </c>
-      <c r="D15" s="96">
+      <c r="D15" s="82">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
@@ -19473,7 +19565,7 @@
       <c r="C16" s="61">
         <v>2</v>
       </c>
-      <c r="D16" s="96">
+      <c r="D16" s="82">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
@@ -19488,16 +19580,16 @@
       <c r="C17" s="61">
         <v>1</v>
       </c>
-      <c r="D17" s="96">
+      <c r="D17" s="82">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="94" t="s">
+      <c r="A18" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="94"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="74"/>
       <c r="D18" s="48">
         <f>SUM(D4:D17)</f>
@@ -19595,10 +19687,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="94"/>
+      <c r="B25" s="96"/>
       <c r="C25" s="74"/>
       <c r="D25" s="48">
         <f>SUM(D19:D24)</f>
@@ -19606,10 +19698,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="94"/>
+      <c r="B26" s="96"/>
       <c r="C26" s="74"/>
       <c r="D26" s="48">
         <f>D18+D25</f>

</xml_diff>